<commit_message>
Giải thích được phần hạn hỷ, tình duyên
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD18B32-F136-4B64-A78E-678A57B62F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237F2D8D-2AC5-4038-A432-5BF8778336A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10292,8 +10292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A2:H2364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2344" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2358" sqref="C2358"/>
+    <sheetView tabSelected="1" topLeftCell="A2359" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2375" sqref="C2375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Giải thích version 2
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237F2D8D-2AC5-4038-A432-5BF8778336A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1A4892-BD14-4255-93FC-26D4BEEA1DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5353" uniqueCount="3269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5354" uniqueCount="3270">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -9887,6 +9887,9 @@
   </si>
   <si>
     <t>Bỏ nhau thì ít nhưng mình dễ mất trước</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Phụ Mẫu tại</t>
   </si>
 </sst>
 </file>
@@ -10290,10 +10293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:H2364"/>
+  <dimension ref="A2:H2365"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2359" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2375" sqref="C2375"/>
+      <selection activeCell="E2361" sqref="E2361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35090,6 +35093,11 @@
       </c>
       <c r="B2364" s="2" t="s">
         <v>3261</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2365" s="2" t="s">
+        <v>3269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải thích hóa quyền ở mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tuvi\TuVi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE0657B-4F56-42EC-B48A-1055972BD70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A1EF48-3CE6-4F66-8C3D-DEADDBE5EC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5387" uniqueCount="3298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10776" uniqueCount="3307">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -10060,6 +10060,33 @@
 - Không coi trọng tiền bạc, thích cùng chia sẻ với mọi người sự thành công.
 - Tự tìm đến sự sầu khổ.
 - Vất vả, nhọc nhằn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vì Hóa Quyền thuộc hỏa, có ý tượng "nâng lên", "biểu hiện một cách rõ ràng" ... Trường hợp Hóa Quyền ở cung mệnh, sẽ làm cho bản thân có tinh thần trách nhiệm và chịu được áp lực, mà mục đích của nó là vì muốn có địa vị xã hội, hoặc để có được sự đồng cảm và phụ họa của người khác.</t>
+  </si>
+  <si>
+    <t>Cung mệnh là hình tượng của một người, cho nên trường hợp có Hóa Quyền ở cung mệnh, dù có quảng bá để nâng bản thân lên thì cũng chỉ là để tạo hình tượng cá nhân, sẽ khiến mệnh tạo có bề ngoài nghiêm túc. Nếu Hóa Lộc và Hóa Kị nhập "ngã cung", thì sẽ có biểu hiện uy nghiêm, uy tín trong lời nói và hành động. Nếu Hóa Lộc và Hóa Kị ở vị trí không thích đáng, hoặc cung mệnh lại tự Hóa Kị, thì sẽ có tính hay ép buộc người khác, khiến cho người ta có cảm giác mệnh tạo là người võ đoán, ỷ thế áp chế người khác, bạo ngược và khó thân cận.</t>
+  </si>
+  <si>
+    <t>Ý tượng của Hóa Quyền có tính thực tiễn, tính thực hiện, tính hành động, biểu hiện của nó đều không ở trạng thái tình. Vì vậy trường hợp Hóa Quyền ở cung mệnh thì khó mà tâm bình khí hòa, tâm cảnh của mệnh tạo khó tĩnh lặng, sẽ có lối suy nghĩ vội vàng, dễ bị kích động, trong lòng hay lo lắng không yên, và hay nhận định một cách hấp tấp.</t>
+  </si>
+  <si>
+    <t>Tứ hóa [năm sinh] ở cung mệnh nhiều ít đều có kiểu suy nghĩ lợi kỉ, hoặc chỉ lo cho mình, bất kể người khác ra sao; mà trường hợp Hóa Quyền là nặng nhất. Hóa Quyền ở cung mệnh, có ưu điểm là tích cực, quyết định và động tác đều mau lẹ, khá chủ quan, ý thức về bản thân rất mạnh, dễ lấy "cái tôi" làm trung tâm, không quan tâm hoặc xem thường lập trường của người khác, tự cho mình là đúng, ngoan cố, khó thông cảm người khác. Hóa Quyền ở cung mệnh, tất nhiên thích nắm quyền, thường có cảm giác mình cao hơn người khác một bậc, sẽ dễ bành trướng "cái tôi", thiếu tính nhẫn nại, không thích nhận lỗi, nhưng cũng nhờ tính cách không chịu thua này mà họ tự đốc thúc bản thân rất mạnh.</t>
+  </si>
+  <si>
+    <t>Trường hợp Hóa Quyền ở cung mệnh thường trưởng thành khá sớm, vì trong đại vận thứ nhất đã có tác động của Hóa Quyền. Lúc còn trẻ đã biết hướng nỗ lực của đời mình, vì vậy khoảng cách cao thấp giữa thành công và thất bại sẽ lớn hơn người bình thường. Nếu Hóa Lộc và Hóa Kị ở ví trí đối nhau thì thành tựu phi phàm, có tính quyền uy. Nếu Hóa Lộc và Hóa Kị ở vị trí không thích đáng thì việc chi ra, hao tổn hơn người bình thường, nhưng lại khó thu hoạch. Hóa Quyền chủ về biến động, sôi nổi; Hóa Quyền ở cung mệnh thì vận trình cuộc đời tất nhiên sẽ nhiều thăng trầm. Nếu bản thân sao Hóa Quyền có tính biến động không yên, hoặc các sao ở cung vị có địa chi xung đột với tính của sao, gặp Hóa Quyền ở cung mệnh, sẽ khó tránh một đời bôn ba, gặp nhiều sóng gió trắc trở, nếm trải đủ thói đời nóng lạnh.</t>
+  </si>
+  <si>
+    <t>Lúc cung mệnh làm cung vị phúc đức của cung phu thê, thì mệnh tạo có tính vội vàng, hấp tấp, dễ bị kích động, sẽ ảnh hưởng đến trạng thái tâm lí của "một nửa kia"; họ luôn muốn dùng thời gian ngắn nhất để tạo ra hiệu quá lớn nhất; sau khi kết hôn, cuộc sống chung của hai người sẽ thấy căng thẳng, cũng không loại trừ trường hợp vì mệnh tạo có tình cảm bên ngoài khiến cho người phối ngẫu phải buồn phiền.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cung mệnh là cầu nối giữa cung phụ mẫu và cung huynh đệ, Hóa Quyền ở cung mệnh, bản thân mệnh tạo là người chủ chốt trong gia đình; nói một cách tương đối, lúc quan hệ giữa cha mẹ và anh em hơi căng thẳng thì mệnh tạo thường là người đứng ra hòa giải.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cung mệnh là cầu nối giữa cung phụ mẫu và cung huynh đệ, Hóa Quyền ở cung mệnh, bản thân mệnh tạo là người chủ chốt trong gia đình; nói một cách tương đối, lúc quan hệ giữa cha mẹ và anh em hơi căng thẳng thì mệnh tạo thường là người đứng ra hòa giải. Tiếp theo trên, nếu lấy cung huynh đệ đại biểu cho mẹ; trường hợp cung phụ mẫu hay cung tật ách có các sao đào hoa, hoặc tổ hợp sao ở cung huynh đệ và cung nô bộc không tốt, thì có thể quan hệ giữa cha và mẹ không được hòa hợp, mà mệnh tạo là cầu nối.</t>
+  </si>
+  <si>
+    <t>Cung mệnh là cung vị điền trạch của cung tử nữ, trường hợp có Hóa Quyền, mệnh tạo có thể là người rất uy nghiêm, khiến con cái ở trong nhà bị áp lực rất nặng, tuy con cái hướng về gia đình, nhưng cũng có phần sợ trong đó, nên ít khi ở nhà</t>
   </si>
 </sst>
 </file>
@@ -10463,10 +10490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:H2381"/>
+  <dimension ref="A2:K2381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2359" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2370" sqref="C2370"/>
+    <sheetView tabSelected="1" topLeftCell="H345" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J353" sqref="J353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10476,6 +10503,9 @@
     <col min="6" max="6" width="51.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="57.42578125" customWidth="1"/>
     <col min="8" max="8" width="59.7109375" customWidth="1"/>
+    <col min="9" max="9" width="48" customWidth="1"/>
+    <col min="10" max="10" width="41.28515625" customWidth="1"/>
+    <col min="11" max="11" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -14147,7 +14177,7 @@
       <c r="F352" s="2"/>
       <c r="G352" s="2"/>
     </row>
-    <row r="353" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>854</v>
       </c>
@@ -14160,7 +14190,7 @@
       <c r="F353" s="2"/>
       <c r="G353" s="2"/>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>855</v>
       </c>
@@ -14170,7 +14200,7 @@
       <c r="F354" s="2"/>
       <c r="G354" s="2"/>
     </row>
-    <row r="355" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>1349</v>
       </c>
@@ -14180,10 +14210,32 @@
       <c r="C355" s="2" t="s">
         <v>2897</v>
       </c>
-      <c r="F355" s="2"/>
-      <c r="G355" s="2"/>
-    </row>
-    <row r="356" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D355" s="2" t="s">
+        <v>3298</v>
+      </c>
+      <c r="E355" s="2" t="s">
+        <v>3299</v>
+      </c>
+      <c r="F355" s="2" t="s">
+        <v>3300</v>
+      </c>
+      <c r="G355" s="2" t="s">
+        <v>3301</v>
+      </c>
+      <c r="H355" s="2" t="s">
+        <v>3302</v>
+      </c>
+      <c r="I355" s="2" t="s">
+        <v>3303</v>
+      </c>
+      <c r="J355" s="2" t="s">
+        <v>3305</v>
+      </c>
+      <c r="K355" s="2" t="s">
+        <v>3306</v>
+      </c>
+    </row>
+    <row r="356" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>1131</v>
       </c>
@@ -14193,7 +14245,7 @@
       <c r="F356" s="2"/>
       <c r="G356" s="2"/>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>873</v>
       </c>
@@ -14203,7 +14255,7 @@
       <c r="F357" s="2"/>
       <c r="G357" s="2"/>
     </row>
-    <row r="358" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>1137</v>
       </c>
@@ -14213,7 +14265,7 @@
       <c r="F358" s="2"/>
       <c r="G358" s="2"/>
     </row>
-    <row r="359" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>747</v>
       </c>
@@ -14223,7 +14275,7 @@
       <c r="F359" s="2"/>
       <c r="G359" s="2"/>
     </row>
-    <row r="360" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>715</v>
       </c>
@@ -14233,7 +14285,7 @@
       <c r="F360" s="2"/>
       <c r="G360" s="2"/>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>746</v>
       </c>
@@ -14243,7 +14295,7 @@
       <c r="F361" s="2"/>
       <c r="G361" s="2"/>
     </row>
-    <row r="362" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>717</v>
       </c>
@@ -14253,7 +14305,7 @@
       <c r="F362" s="2"/>
       <c r="G362" s="2"/>
     </row>
-    <row r="363" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>731</v>
       </c>
@@ -14263,7 +14315,7 @@
       <c r="F363" s="2"/>
       <c r="G363" s="2"/>
     </row>
-    <row r="364" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>733</v>
       </c>
@@ -14273,7 +14325,7 @@
       <c r="F364" s="2"/>
       <c r="G364" s="2"/>
     </row>
-    <row r="365" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>750</v>
       </c>
@@ -14283,7 +14335,7 @@
       <c r="F365" s="2"/>
       <c r="G365" s="2"/>
     </row>
-    <row r="366" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>719</v>
       </c>
@@ -14293,7 +14345,7 @@
       <c r="F366" s="2"/>
       <c r="G366" s="2"/>
     </row>
-    <row r="367" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>737</v>
       </c>
@@ -14303,7 +14355,7 @@
       <c r="F367" s="2"/>
       <c r="G367" s="2"/>
     </row>
-    <row r="368" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>725</v>
       </c>

</xml_diff>